<commit_message>
Completed CS import functionality
</commit_message>
<xml_diff>
--- a/Data/Charles Stanley test import.xlsx
+++ b/Data/Charles Stanley test import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Portfolio-management\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851370F0-8BE1-4314-A29D-4DA90839A339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C811A3-EB61-4FE2-B354-858A355F769F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="58">
   <si>
     <t>Account Name</t>
   </si>
@@ -85,10 +85,67 @@
     <t>Balance</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t>Important Information</t>
+  </si>
+  <si>
+    <t>Charles Stanley Direct is a trading name of Charles Stanley &amp; Co. Limited. Registered in England No 1903304. Registered Office: Ropemaker Place, 25 Ropemaker Street, London EC2Y 9LY. Authorised and regulated by the Financial Conduct Authority (No. 124412). Member of the London Stock Exchange.</t>
+  </si>
+  <si>
+    <t>Investors should be aware that past performance is not a reliable indicator of future results and that the price of shares and other investments, and the income derived from them, may fall as well as rise and the amount realised may be less than the original sum invested.</t>
+  </si>
+  <si>
+    <t>Transfer to capital account</t>
+  </si>
+  <si>
+    <t>Transfer from Div Ac</t>
+  </si>
+  <si>
+    <t>10-Apr-2014</t>
+  </si>
+  <si>
+    <t>01-Apr-2014</t>
+  </si>
+  <si>
+    <t>Gross interest to 31/03/14</t>
+  </si>
+  <si>
+    <t>22-Apr-2015</t>
+  </si>
+  <si>
+    <t>2367.648 FIL INV  Del    1.05 S Date 28/04/15</t>
+  </si>
+  <si>
+    <t>BLT1YQ4</t>
+  </si>
+  <si>
+    <t>FIL INV SVCS UK INDEX EURP EX UK W ACC NAV</t>
+  </si>
+  <si>
+    <t>I96587</t>
+  </si>
+  <si>
+    <t>28-Apr-2015</t>
+  </si>
+  <si>
     <t>Funds Platform Fee</t>
   </si>
   <si>
-    <t/>
+    <t>Stocks &amp; Shares Subs</t>
+  </si>
+  <si>
+    <t>03-Feb-2015</t>
+  </si>
+  <si>
+    <t>26-Jan-2015</t>
+  </si>
+  <si>
+    <t>30-Jan-2015</t>
+  </si>
+  <si>
+    <t>6.755 VAN FTSE DEV  Del  222.05 S Date 30/01/15</t>
   </si>
   <si>
     <t>B59G4Q7</t>
@@ -97,24 +154,12 @@
     <t>VANGUARD INV UK LT FTSE DEVELOPED WLD EX UK EQ</t>
   </si>
   <si>
-    <t>Stocks &amp; Shares Subs</t>
-  </si>
-  <si>
-    <t>03-Feb-2015</t>
-  </si>
-  <si>
-    <t>26-Jan-2015</t>
-  </si>
-  <si>
-    <t>30-Jan-2015</t>
-  </si>
-  <si>
-    <t>6.755 VAN FTSE DEV  Del  222.05 S Date 30/01/15</t>
-  </si>
-  <si>
     <t>F39873</t>
   </si>
   <si>
+    <t>Govt Flat Rate Int Charge</t>
+  </si>
+  <si>
     <t>24-Mar-2014</t>
   </si>
   <si>
@@ -124,13 +169,31 @@
     <t>* BALANCE B/F *</t>
   </si>
   <si>
-    <t>Important Information</t>
-  </si>
-  <si>
-    <t>Charles Stanley Direct is a trading name of Charles Stanley &amp; Co. Limited. Registered in England No 1903304. Registered Office: Ropemaker Place, 25 Ropemaker Street, London EC2Y 9LY. Authorised and regulated by the Financial Conduct Authority (No. 124412). Member of the London Stock Exchange.</t>
-  </si>
-  <si>
-    <t>Investors should be aware that past performance is not a reliable indicator of future results and that the price of shares and other investments, and the income derived from them, may fall as well as rise and the amount realised may be less than the original sum invested.</t>
+    <t>25-May-2018</t>
+  </si>
+  <si>
+    <t>10.309 VAN FTSE DEV  Del  339.50 S Date 30/05/18</t>
+  </si>
+  <si>
+    <t>X30545</t>
+  </si>
+  <si>
+    <t>30-May-2018</t>
+  </si>
+  <si>
+    <t>08-Oct-2018</t>
+  </si>
+  <si>
+    <t>BACS P'MNT          ****6919</t>
+  </si>
+  <si>
+    <t>15-Nov-2021</t>
+  </si>
+  <si>
+    <t>Dividend Grp 1 85.52 BARS INV</t>
+  </si>
+  <si>
+    <t>BG7PJH9</t>
   </si>
 </sst>
 </file>
@@ -189,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -204,24 +267,18 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -587,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J146"/>
+  <dimension ref="A1:J154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B5" sqref="A5:XFD5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
@@ -608,9 +665,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="6"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
@@ -631,9 +688,9 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
       <c r="D2" t="s">
         <v>6</v>
       </c>
@@ -654,9 +711,9 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="4" t="s">
@@ -692,51 +749,51 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F5" s="3">
         <v>0</v>
       </c>
       <c r="G5" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>0</v>
       </c>
       <c r="H5" s="3">
-        <v>0</v>
+        <v>22.98</v>
       </c>
       <c r="J5" s="3">
-        <v>8021.36</v>
+        <v>34.22</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="F6" s="3">
-        <v>222.05625000000001</v>
+        <v>0</v>
       </c>
       <c r="G6" s="3">
         <v>1500</v>
@@ -744,343 +801,525 @@
       <c r="H6" s="3">
         <v>0</v>
       </c>
-      <c r="I6" t="s">
-        <v>28</v>
-      </c>
       <c r="J6" s="3">
-        <v>10021.43</v>
+        <v>5255.39</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="F7" s="3">
-        <v>0</v>
+        <v>339.50916000000001</v>
       </c>
       <c r="G7" s="3">
-        <v>0</v>
+        <v>3500</v>
       </c>
       <c r="H7" s="3">
-        <v>11520</v>
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>52</v>
       </c>
       <c r="J7" s="3">
-        <v>11520</v>
+        <v>6776.32</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
         <v>32</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8" t="s">
         <v>33</v>
       </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
       <c r="E8" s="2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="F8" s="3">
-        <v>0</v>
+        <v>1.0558799999999999</v>
       </c>
       <c r="G8" s="3">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="H8" s="3">
         <v>0</v>
       </c>
+      <c r="I8" t="s">
+        <v>35</v>
+      </c>
       <c r="J8" s="3">
-        <v>0</v>
+        <v>20521.39</v>
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="J9" s="3"/>
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3">
+        <v>8021.36</v>
+      </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="E10" s="2"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="J10" s="3"/>
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="3">
+        <v>222.05625000000001</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1500</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10" s="3">
+        <v>10021.43</v>
+      </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="E11" s="2"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="J11" s="3"/>
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0.11</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
+      <c r="J11" s="3">
+        <v>11520.11</v>
+      </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="B12" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="J12" s="9" t="s">
-        <v>34</v>
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0.11</v>
+      </c>
+      <c r="J12" s="3">
+        <v>11520.22</v>
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="B13" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="I13" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>35</v>
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0.13</v>
+      </c>
+      <c r="J13" s="3">
+        <v>11520.11</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="B14" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="J14" s="11" t="s">
-        <v>35</v>
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
+      <c r="J14" s="3">
+        <v>11519.98</v>
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="B15" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="H15" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="I15" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="J15" s="13" t="s">
-        <v>36</v>
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3">
+        <v>11520</v>
+      </c>
+      <c r="J15" s="3">
+        <v>11520</v>
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="B16" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="H16" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="I16" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="J16" s="13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="5:10">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0</v>
+      </c>
+      <c r="H16" s="3">
+        <v>0</v>
+      </c>
+      <c r="J16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10">
       <c r="E17" s="2"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="5:10">
+    <row r="18" spans="2:10">
       <c r="E18" s="2"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="J18" s="3"/>
     </row>
-    <row r="19" spans="5:10">
+    <row r="19" spans="2:10">
       <c r="E19" s="2"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="5:10">
-      <c r="E20" s="2"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="J20" s="3"/>
-    </row>
-    <row r="21" spans="5:10">
-      <c r="E21" s="2"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="J21" s="3"/>
-    </row>
-    <row r="22" spans="5:10">
-      <c r="E22" s="2"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="J22" s="3"/>
-    </row>
-    <row r="23" spans="5:10">
-      <c r="E23" s="2"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="J23" s="3"/>
-    </row>
-    <row r="24" spans="5:10">
-      <c r="E24" s="2"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="J24" s="3"/>
-    </row>
-    <row r="25" spans="5:10">
+    <row r="20" spans="2:10">
+      <c r="B20" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10">
+      <c r="B21" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I21" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J21" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10">
+      <c r="B22" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J22" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10">
+      <c r="B23" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I23" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="J23" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10">
+      <c r="B24" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="J24" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10">
       <c r="E25" s="2"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="J25" s="3"/>
     </row>
-    <row r="26" spans="5:10">
+    <row r="26" spans="2:10">
       <c r="E26" s="2"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="J26" s="3"/>
     </row>
-    <row r="27" spans="5:10">
+    <row r="27" spans="2:10">
       <c r="E27" s="2"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="J27" s="3"/>
     </row>
-    <row r="28" spans="5:10">
+    <row r="28" spans="2:10">
       <c r="E28" s="2"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="J28" s="3"/>
     </row>
-    <row r="29" spans="5:10">
+    <row r="29" spans="2:10">
       <c r="E29" s="2"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="J29" s="3"/>
     </row>
-    <row r="30" spans="5:10">
+    <row r="30" spans="2:10">
       <c r="E30" s="2"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="J30" s="3"/>
     </row>
-    <row r="31" spans="5:10">
+    <row r="31" spans="2:10">
       <c r="E31" s="2"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="J31" s="3"/>
     </row>
-    <row r="32" spans="5:10">
+    <row r="32" spans="2:10">
       <c r="E32" s="2"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
@@ -1885,12 +2124,67 @@
       <c r="H146" s="3"/>
       <c r="J146" s="3"/>
     </row>
+    <row r="147" spans="5:10">
+      <c r="E147" s="2"/>
+      <c r="F147" s="3"/>
+      <c r="G147" s="3"/>
+      <c r="H147" s="3"/>
+      <c r="J147" s="3"/>
+    </row>
+    <row r="148" spans="5:10">
+      <c r="E148" s="2"/>
+      <c r="F148" s="3"/>
+      <c r="G148" s="3"/>
+      <c r="H148" s="3"/>
+      <c r="J148" s="3"/>
+    </row>
+    <row r="149" spans="5:10">
+      <c r="E149" s="2"/>
+      <c r="F149" s="3"/>
+      <c r="G149" s="3"/>
+      <c r="H149" s="3"/>
+      <c r="J149" s="3"/>
+    </row>
+    <row r="150" spans="5:10">
+      <c r="E150" s="2"/>
+      <c r="F150" s="3"/>
+      <c r="G150" s="3"/>
+      <c r="H150" s="3"/>
+      <c r="J150" s="3"/>
+    </row>
+    <row r="151" spans="5:10">
+      <c r="E151" s="2"/>
+      <c r="F151" s="3"/>
+      <c r="G151" s="3"/>
+      <c r="H151" s="3"/>
+      <c r="J151" s="3"/>
+    </row>
+    <row r="152" spans="5:10">
+      <c r="E152" s="2"/>
+      <c r="F152" s="3"/>
+      <c r="G152" s="3"/>
+      <c r="H152" s="3"/>
+      <c r="J152" s="3"/>
+    </row>
+    <row r="153" spans="5:10">
+      <c r="E153" s="2"/>
+      <c r="F153" s="3"/>
+      <c r="G153" s="3"/>
+      <c r="H153" s="3"/>
+      <c r="J153" s="3"/>
+    </row>
+    <row r="154" spans="5:10">
+      <c r="E154" s="2"/>
+      <c r="F154" s="3"/>
+      <c r="G154" s="3"/>
+      <c r="H154" s="3"/>
+      <c r="J154" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A1:C3"/>
-    <mergeCell ref="B12:J12"/>
-    <mergeCell ref="B13:J14"/>
-    <mergeCell ref="B15:J16"/>
+    <mergeCell ref="B21:J22"/>
+    <mergeCell ref="B23:J24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter differentOddEven="1">

</xml_diff>